<commit_message>
Fixed bug with double to int conversion in minimax
</commit_message>
<xml_diff>
--- a/results/AI vs AI.xlsx
+++ b/results/AI vs AI.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t xml:space="preserve">Heuristics: </t>
   </si>
@@ -44,9 +45,6 @@
     <t>reinforcement</t>
   </si>
   <si>
-    <t>count_diff + score_diff + moves_diff + reinf_diff</t>
-  </si>
-  <si>
     <t>AI #2</t>
   </si>
   <si>
@@ -102,6 +100,15 @@
   </si>
   <si>
     <t>neighbors difference</t>
+  </si>
+  <si>
+    <t>1+2+3.5</t>
+  </si>
+  <si>
+    <t>1+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must be an error with the depth being so low. </t>
   </si>
 </sst>
 </file>
@@ -456,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -511,7 +518,7 @@
         <v>3.2</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -519,7 +526,7 @@
         <v>3.3</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -527,7 +534,7 @@
         <v>3.4</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -535,7 +542,7 @@
         <v>3.5</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -543,7 +550,7 @@
         <v>3.6</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -554,44 +561,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
       <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
         <v>13</v>
       </c>
-      <c r="H18" t="s">
-        <v>14</v>
-      </c>
       <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" t="s">
         <v>11</v>
-      </c>
-      <c r="J18" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1063,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E35">
         <v>200</v>
@@ -1092,22 +1094,19 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E36">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="G36">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="H36">
-        <v>185</v>
+        <v>447</v>
       </c>
       <c r="I36">
-        <v>17.73</v>
-      </c>
-      <c r="J36">
-        <v>45.95</v>
+        <v>19.100000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1118,25 +1117,25 @@
         <v>10</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E37">
         <v>200</v>
       </c>
       <c r="G37">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H37">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I37">
-        <v>17.28</v>
+        <v>17.73</v>
       </c>
       <c r="J37">
-        <v>46.5</v>
+        <v>45.95</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1150,22 +1149,22 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E38">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="G38">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="H38">
-        <v>456</v>
+        <v>189</v>
       </c>
       <c r="I38">
-        <v>19.28</v>
+        <v>17.28</v>
       </c>
       <c r="J38">
-        <v>44.61</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1176,28 +1175,25 @@
         <v>10</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E39">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="G39">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="H39">
-        <v>193</v>
+        <v>456</v>
       </c>
       <c r="I39">
-        <v>19.399999999999999</v>
+        <v>19.28</v>
       </c>
       <c r="J39">
-        <v>44.6</v>
-      </c>
-      <c r="L39" t="s">
-        <v>16</v>
+        <v>44.61</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1207,26 +1203,29 @@
       <c r="B40">
         <v>10</v>
       </c>
-      <c r="C40" t="s">
-        <v>17</v>
+      <c r="C40">
+        <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E40">
         <v>200</v>
       </c>
       <c r="G40">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="H40">
-        <v>119</v>
+        <v>193</v>
       </c>
       <c r="I40">
-        <v>28.71</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="J40">
-        <v>35.25</v>
+        <v>44.6</v>
+      </c>
+      <c r="L40" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1236,8 +1235,8 @@
       <c r="B41">
         <v>10</v>
       </c>
-      <c r="C41">
-        <v>2</v>
+      <c r="C41" t="s">
+        <v>16</v>
       </c>
       <c r="D41" t="s">
         <v>18</v>
@@ -1246,16 +1245,338 @@
         <v>200</v>
       </c>
       <c r="G41">
+        <v>73</v>
+      </c>
+      <c r="H41">
+        <v>119</v>
+      </c>
+      <c r="I41">
+        <v>28.71</v>
+      </c>
+      <c r="J41">
+        <v>35.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42">
+        <v>200</v>
+      </c>
+      <c r="G42">
         <v>134</v>
       </c>
-      <c r="H41">
+      <c r="H42">
         <v>65</v>
       </c>
-      <c r="I41">
+      <c r="I42">
         <v>32.79</v>
       </c>
-      <c r="J41">
+      <c r="J42">
         <v>31.21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43">
+        <v>200</v>
+      </c>
+      <c r="G43">
+        <v>11</v>
+      </c>
+      <c r="H43">
+        <v>187</v>
+      </c>
+      <c r="I43">
+        <v>17.43</v>
+      </c>
+      <c r="J43">
+        <v>46.57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47">
+        <v>200</v>
+      </c>
+      <c r="G47">
+        <v>20</v>
+      </c>
+      <c r="H47">
+        <v>177</v>
+      </c>
+      <c r="I47">
+        <v>20.3</v>
+      </c>
+      <c r="J47">
+        <v>40.229999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48">
+        <v>100</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48">
+        <v>95</v>
+      </c>
+      <c r="I48">
+        <v>18.09</v>
+      </c>
+      <c r="J48">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49">
+        <v>200</v>
+      </c>
+      <c r="G49">
+        <v>11</v>
+      </c>
+      <c r="H49">
+        <v>188</v>
+      </c>
+      <c r="I49">
+        <v>17.670000000000002</v>
+      </c>
+      <c r="J49">
+        <v>46.31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50">
+        <v>100</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>96</v>
+      </c>
+      <c r="I50">
+        <v>16.18</v>
+      </c>
+      <c r="J50">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51">
+        <v>10</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>10</v>
+      </c>
+      <c r="I51">
+        <v>14.9</v>
+      </c>
+      <c r="J51">
+        <v>49.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>10</v>
+      </c>
+      <c r="C52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52">
+        <v>10</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>10</v>
+      </c>
+      <c r="I52">
+        <v>21.7</v>
+      </c>
+      <c r="J52">
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53">
+        <v>200</v>
+      </c>
+      <c r="G53">
+        <v>170</v>
+      </c>
+      <c r="H53">
+        <v>30</v>
+      </c>
+      <c r="I53">
+        <v>42.34</v>
+      </c>
+      <c r="J53">
+        <v>21.7</v>
+      </c>
+      <c r="L53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>10</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54">
+        <v>200</v>
+      </c>
+      <c r="G54">
+        <v>105</v>
+      </c>
+      <c r="H54">
+        <v>93</v>
+      </c>
+      <c r="I54">
+        <v>35.08</v>
+      </c>
+      <c r="J54">
+        <v>28.92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>10</v>
+      </c>
+      <c r="C55" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55">
+        <v>50</v>
+      </c>
+      <c r="G55">
+        <v>18</v>
+      </c>
+      <c r="H55">
+        <v>32</v>
+      </c>
+      <c r="I55">
+        <v>31.5</v>
+      </c>
+      <c r="J55">
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced Minimax with Negamax
</commit_message>
<xml_diff>
--- a/results/AI vs AI.xlsx
+++ b/results/AI vs AI.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
   <si>
     <t xml:space="preserve">Heuristics: </t>
   </si>
@@ -109,6 +108,15 @@
   </si>
   <si>
     <t xml:space="preserve">Must be an error with the depth being so low. </t>
+  </si>
+  <si>
+    <t>Tree type</t>
+  </si>
+  <si>
+    <t>Minimax</t>
+  </si>
+  <si>
+    <t>Negamax</t>
   </si>
 </sst>
 </file>
@@ -463,17 +471,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.41796875" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="4" max="4" width="10.5234375" customWidth="1"/>
+    <col min="2" max="2" width="11.41796875" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="5" max="5" width="10.5234375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -561,1027 +569,1262 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="1" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
         <v>8</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>6</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>9</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>12</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>13</v>
       </c>
-      <c r="I18" t="s">
-        <v>10</v>
-      </c>
       <c r="J18" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
-        <v>2</v>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>29</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>200</v>
-      </c>
-      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>200</v>
+      </c>
+      <c r="H19">
         <v>111</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>83</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>32.799999999999997</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>31.2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
-        <v>2</v>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>29</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
-      <c r="E20">
-        <v>200</v>
-      </c>
-      <c r="G20">
+      <c r="F20">
+        <v>200</v>
+      </c>
+      <c r="H20">
         <v>67</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>124</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>27.93</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>35.65</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
-        <v>2</v>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>29</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>200</v>
-      </c>
-      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>200</v>
+      </c>
+      <c r="H21">
         <v>19</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>180</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>21.55</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>40.78</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
-        <v>2</v>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>29</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>3.1</v>
       </c>
-      <c r="E22">
-        <v>200</v>
-      </c>
-      <c r="G22">
+      <c r="F22">
+        <v>200</v>
+      </c>
+      <c r="H22">
         <v>62</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>136</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>25.85</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>38.11</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23">
-        <v>2</v>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>29</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
         <v>3.1</v>
       </c>
-      <c r="E23">
-        <v>200</v>
-      </c>
-      <c r="G23">
+      <c r="F23">
+        <v>200</v>
+      </c>
+      <c r="H23">
         <v>54</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24">
-        <v>2</v>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>29</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
         <v>3.2</v>
       </c>
-      <c r="E24">
-        <v>200</v>
-      </c>
-      <c r="G24">
+      <c r="F24">
+        <v>200</v>
+      </c>
+      <c r="H24">
         <v>53</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>139</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>25.225000000000001</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>38.71</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25">
-        <v>2</v>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>29</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
         <v>3.2</v>
       </c>
-      <c r="E25">
-        <v>200</v>
-      </c>
-      <c r="G25">
+      <c r="F25">
+        <v>200</v>
+      </c>
+      <c r="H25">
         <v>44</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>153</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>23.204999999999998</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>40.770000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26">
-        <v>2</v>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>29</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
         <v>3.2</v>
       </c>
-      <c r="E26">
-        <v>200</v>
-      </c>
-      <c r="G26">
+      <c r="F26">
+        <v>200</v>
+      </c>
+      <c r="H26">
         <v>54</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>144</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>24.66</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>39.08</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
         <v>3</v>
       </c>
-      <c r="B27">
-        <v>10</v>
-      </c>
       <c r="C27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>3.2</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>50</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>9</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>38</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>23.68</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>40.28</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28">
-        <v>2</v>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
         <v>3.3</v>
       </c>
-      <c r="E28">
-        <v>200</v>
-      </c>
-      <c r="G28">
+      <c r="F28">
+        <v>200</v>
+      </c>
+      <c r="H28">
         <v>53</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>141</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>25.44</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>38.56</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29">
-        <v>2</v>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
         <v>3.4</v>
       </c>
-      <c r="E29">
-        <v>200</v>
-      </c>
-      <c r="G29">
+      <c r="F29">
+        <v>200</v>
+      </c>
+      <c r="H29">
         <v>79</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>118</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>29.305</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>34.549999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30">
-        <v>2</v>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>3.5</v>
       </c>
-      <c r="E30">
-        <v>200</v>
-      </c>
-      <c r="G30">
+      <c r="F30">
+        <v>200</v>
+      </c>
+      <c r="H30">
         <v>48</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>146</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>25.6</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>38.36</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31">
-        <v>2</v>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
         <v>3.6</v>
       </c>
-      <c r="E31">
-        <v>200</v>
-      </c>
-      <c r="G31">
+      <c r="F31">
+        <v>200</v>
+      </c>
+      <c r="H31">
         <v>70</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>124</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>26.71</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>37.204999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32">
-        <v>2</v>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>29</v>
       </c>
       <c r="B32">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
         <v>4</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>400</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>211</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>175</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>33</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>30.99</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33">
-        <v>2</v>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>29</v>
       </c>
       <c r="B33">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
         <v>1</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>4</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>100</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>64</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>31</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>37.130000000000003</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>26.86</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34">
-        <v>2</v>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>29</v>
       </c>
       <c r="B34">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
         <v>1</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>4</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>300</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>214</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>80</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>37.270000000000003</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>26.14</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35">
-        <v>2</v>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>29</v>
       </c>
       <c r="B35">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
         <v>17</v>
       </c>
-      <c r="E35">
-        <v>200</v>
-      </c>
-      <c r="G35">
+      <c r="F35">
+        <v>200</v>
+      </c>
+      <c r="H35">
         <v>7</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>193</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>17.3</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>46.66</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36">
-        <v>2</v>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>29</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
         <v>17</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>500</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>47</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>447</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37">
-        <v>2</v>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>29</v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
         <v>18</v>
       </c>
-      <c r="E37">
-        <v>200</v>
-      </c>
-      <c r="G37">
+      <c r="F37">
+        <v>200</v>
+      </c>
+      <c r="H37">
         <v>15</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>185</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>17.73</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>45.95</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38">
-        <v>2</v>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>29</v>
       </c>
       <c r="B38">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
         <v>1</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>18</v>
       </c>
-      <c r="E38">
-        <v>200</v>
-      </c>
-      <c r="G38">
+      <c r="F38">
+        <v>200</v>
+      </c>
+      <c r="H38">
         <v>7</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>189</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>17.28</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>46.5</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39">
-        <v>2</v>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>29</v>
       </c>
       <c r="B39">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39">
         <v>1</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>18</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>500</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>39</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>456</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>19.28</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>44.61</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40">
-        <v>2</v>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>29</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
         <v>18</v>
       </c>
-      <c r="E40">
-        <v>200</v>
-      </c>
-      <c r="G40">
+      <c r="F40">
+        <v>200</v>
+      </c>
+      <c r="H40">
         <v>4</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>193</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>19.399999999999999</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>44.6</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41">
-        <v>2</v>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>29</v>
       </c>
       <c r="B41">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
         <v>16</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>18</v>
       </c>
-      <c r="E41">
-        <v>200</v>
-      </c>
-      <c r="G41">
+      <c r="F41">
+        <v>200</v>
+      </c>
+      <c r="H41">
         <v>73</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>119</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>28.71</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>35.25</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42">
-        <v>2</v>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>29</v>
       </c>
       <c r="B42">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
         <v>17</v>
       </c>
-      <c r="E42">
-        <v>200</v>
-      </c>
-      <c r="G42">
+      <c r="F42">
+        <v>200</v>
+      </c>
+      <c r="H42">
         <v>134</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>65</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>32.79</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>31.21</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43">
         <v>4</v>
       </c>
-      <c r="B43">
-        <v>10</v>
-      </c>
       <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
         <v>25</v>
       </c>
-      <c r="E43">
-        <v>200</v>
-      </c>
-      <c r="G43">
+      <c r="F43">
+        <v>200</v>
+      </c>
+      <c r="H43">
         <v>11</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>187</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>17.43</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>46.57</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47">
-        <v>2</v>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>29</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
         <v>26</v>
       </c>
-      <c r="E47">
-        <v>200</v>
-      </c>
-      <c r="G47">
+      <c r="F47">
+        <v>200</v>
+      </c>
+      <c r="H47">
         <v>20</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>177</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>20.3</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>40.229999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48">
         <v>4</v>
       </c>
-      <c r="B48">
-        <v>10</v>
-      </c>
       <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
         <v>26</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>100</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>5</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>95</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>18.09</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49">
-        <v>2</v>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>29</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
         <v>25</v>
       </c>
-      <c r="E49">
-        <v>200</v>
-      </c>
-      <c r="G49">
+      <c r="F49">
+        <v>200</v>
+      </c>
+      <c r="H49">
         <v>11</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>188</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>17.670000000000002</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>46.31</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50">
         <v>4</v>
       </c>
-      <c r="B50">
-        <v>10</v>
-      </c>
       <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
         <v>25</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>100</v>
       </c>
-      <c r="G50">
-        <v>2</v>
-      </c>
       <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
         <v>96</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>16.18</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>47.8</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51">
         <v>5</v>
       </c>
-      <c r="B51">
-        <v>10</v>
-      </c>
       <c r="C51">
-        <v>0</v>
-      </c>
-      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
         <v>25</v>
       </c>
-      <c r="E51">
-        <v>10</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
+      <c r="F51">
+        <v>10</v>
       </c>
       <c r="H51">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I51">
+        <v>10</v>
+      </c>
+      <c r="J51">
         <v>14.9</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>49.1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52">
         <v>4</v>
       </c>
-      <c r="B52">
-        <v>10</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
         <v>26</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>25</v>
       </c>
-      <c r="E52">
-        <v>10</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
+      <c r="F52">
+        <v>10</v>
       </c>
       <c r="H52">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I52">
+        <v>10</v>
+      </c>
+      <c r="J52">
         <v>21.7</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>42.3</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53">
-        <v>2</v>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>29</v>
       </c>
       <c r="B53">
-        <v>10</v>
-      </c>
-      <c r="C53" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
       </c>
       <c r="D53" t="s">
         <v>25</v>
       </c>
-      <c r="E53">
-        <v>200</v>
-      </c>
-      <c r="G53">
+      <c r="E53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53">
+        <v>200</v>
+      </c>
+      <c r="H53">
         <v>170</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>30</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>42.34</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>21.7</v>
       </c>
-      <c r="L53" t="s">
+      <c r="M53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54">
         <v>3</v>
       </c>
-      <c r="B54">
-        <v>10</v>
-      </c>
-      <c r="C54" t="s">
-        <v>25</v>
+      <c r="C54">
+        <v>10</v>
       </c>
       <c r="D54" t="s">
         <v>25</v>
       </c>
-      <c r="E54">
-        <v>200</v>
-      </c>
-      <c r="G54">
+      <c r="E54" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54">
+        <v>200</v>
+      </c>
+      <c r="H54">
         <v>105</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>93</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>35.08</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>28.92</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55">
         <v>4</v>
       </c>
-      <c r="B55">
-        <v>10</v>
-      </c>
-      <c r="C55" t="s">
-        <v>25</v>
+      <c r="C55">
+        <v>10</v>
       </c>
       <c r="D55" t="s">
         <v>25</v>
       </c>
-      <c r="E55">
+      <c r="E55" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55">
         <v>50</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>18</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>32</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>31.5</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>32.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>200</v>
+      </c>
+      <c r="H57">
+        <v>35</v>
+      </c>
+      <c r="I57">
+        <v>158</v>
+      </c>
+      <c r="J57">
+        <v>23.8</v>
+      </c>
+      <c r="K57">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58">
+        <v>20</v>
+      </c>
+      <c r="I58">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>10</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <v>200</v>
+      </c>
+      <c r="H59">
+        <v>25</v>
+      </c>
+      <c r="I59">
+        <v>170</v>
+      </c>
+      <c r="J59">
+        <v>21.8</v>
+      </c>
+      <c r="K59">
+        <v>40.72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>200</v>
+      </c>
+      <c r="H60">
+        <v>18</v>
+      </c>
+      <c r="I60">
+        <v>174</v>
+      </c>
+      <c r="J60">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="K60">
+        <v>41.03</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Introduced Stability and potential mobility heuristics
</commit_message>
<xml_diff>
--- a/results/AI vs AI.xlsx
+++ b/results/AI vs AI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
   <si>
     <t xml:space="preserve">Heuristics: </t>
   </si>
@@ -471,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1708,34 +1708,55 @@
       <c r="D57">
         <v>0</v>
       </c>
-      <c r="E57">
-        <v>2</v>
+      <c r="E57" t="s">
+        <v>25</v>
       </c>
       <c r="F57">
         <v>200</v>
       </c>
       <c r="H57">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="I57">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="J57">
-        <v>23.8</v>
+        <v>20.149999999999999</v>
       </c>
       <c r="K57">
-        <v>40</v>
+        <v>43.83</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>30</v>
       </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>10</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58">
+        <v>200</v>
+      </c>
       <c r="H58">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I58">
-        <v>174</v>
+        <v>182</v>
+      </c>
+      <c r="J58">
+        <v>18.62</v>
+      </c>
+      <c r="K58">
+        <v>45.32</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1743,31 +1764,31 @@
         <v>30</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C59">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
-      <c r="E59">
-        <v>2</v>
+      <c r="E59" t="s">
+        <v>25</v>
       </c>
       <c r="F59">
         <v>200</v>
       </c>
       <c r="H59">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I59">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="J59">
-        <v>21.8</v>
+        <v>19.5</v>
       </c>
       <c r="K59">
-        <v>40.72</v>
+        <v>44.45</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1775,31 +1796,31 @@
         <v>30</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C60">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
-      <c r="E60">
-        <v>2</v>
+      <c r="E60" t="s">
+        <v>25</v>
       </c>
       <c r="F60">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H60">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I60">
-        <v>174</v>
+        <v>85</v>
       </c>
       <c r="J60">
-        <v>19.899999999999999</v>
+        <v>20.29</v>
       </c>
       <c r="K60">
-        <v>41.03</v>
+        <v>43.7</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1807,19 +1828,60 @@
         <v>30</v>
       </c>
       <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>25</v>
+      </c>
+      <c r="F61">
+        <v>10</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>10</v>
+      </c>
+      <c r="J61">
+        <v>17.8</v>
+      </c>
+      <c r="K61">
+        <v>46.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62">
         <v>3</v>
       </c>
-      <c r="C61">
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
         <v>3</v>
       </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>2</v>
-      </c>
-      <c r="F61">
-        <v>200</v>
+      <c r="J62">
+        <v>22</v>
+      </c>
+      <c r="K62">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dynamic heuristic function
</commit_message>
<xml_diff>
--- a/results/AI vs AI.xlsx
+++ b/results/AI vs AI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="34">
   <si>
     <t xml:space="preserve">Heuristics: </t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>Negamax</t>
+  </si>
+  <si>
+    <t>1,2,10,1,3,1</t>
+  </si>
+  <si>
+    <t>1,1,10,1,3,1</t>
+  </si>
+  <si>
+    <t>0.5,1,10,1,3,1</t>
   </si>
 </sst>
 </file>
@@ -471,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="L62" sqref="L62"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1884,6 +1893,113 @@
         <v>42</v>
       </c>
     </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>31</v>
+      </c>
+      <c r="F65">
+        <v>1000</v>
+      </c>
+      <c r="H65">
+        <v>82</v>
+      </c>
+      <c r="I65">
+        <v>897</v>
+      </c>
+      <c r="J65">
+        <v>19.12</v>
+      </c>
+      <c r="K65">
+        <v>44.69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>32</v>
+      </c>
+      <c r="F66">
+        <v>1000</v>
+      </c>
+      <c r="H66">
+        <v>79</v>
+      </c>
+      <c r="I66">
+        <v>914</v>
+      </c>
+      <c r="J66">
+        <v>18.661999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67">
+        <v>1000</v>
+      </c>
+      <c r="H67">
+        <v>106</v>
+      </c>
+      <c r="I67">
+        <v>875</v>
+      </c>
+      <c r="J67">
+        <v>20</v>
+      </c>
+      <c r="K67">
+        <v>44.01</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D17:E17"/>

</xml_diff>